<commit_message>
Ready for production v-1
</commit_message>
<xml_diff>
--- a/Reviews.xlsx
+++ b/Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AudibleHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E624BAE1-E188-4178-BADD-994478E888D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923CBE3E-3E3B-41B6-AE62-14BAD59F7324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Chester robin</t>
+    <t>Mcintosh</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,11 +383,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>43749</v>
+        <v>43765</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.audible.co.uk/listener/A89XFJ7UQTS9L?pf_rd_p=d85bb0c7-d987-483d-acca-afcf5c6bc241&amp;pf_rd_r=7WM9F89SZSBNP94R9B4V&amp;ref=a_pd_Anger-_c16_rvlsnl_0" xr:uid="{D9198405-EC1F-4C92-B857-172F4A4A4981}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing for dontet core 2.1
</commit_message>
<xml_diff>
--- a/Reviews.xlsx
+++ b/Reviews.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AudibleHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923CBE3E-3E3B-41B6-AE62-14BAD59F7324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF45DCC5-01EB-43EA-8C75-BC14C6375D99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -33,14 +33,26 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Mcintosh</t>
+    <t>Ellen</t>
+  </si>
+  <si>
+    <t>Wilbert</t>
+  </si>
+  <si>
+    <t>Josie</t>
+  </si>
+  <si>
+    <t>Marcy</t>
+  </si>
+  <si>
+    <t>Carmine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +66,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,13 +94,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,19 +399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,20 +419,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>43765</v>
+        <v>43779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43779</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.audible.co.uk/listener/A89XFJ7UQTS9L?pf_rd_p=d85bb0c7-d987-483d-acca-afcf5c6bc241&amp;pf_rd_r=7WM9F89SZSBNP94R9B4V&amp;ref=a_pd_Anger-_c16_rvlsnl_0" xr:uid="{D9198405-EC1F-4C92-B857-172F4A4A4981}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>